<commit_message>
Added List for multiple product
Enable it retireve multiple pricing based on the number of product it has  in the productUrl list that is appened to.
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5805" yWindow="1530" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -428,13 +428,30 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Test1</t>
+          <t>Badland</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="F4" t="n">
-        <v>3.14</v>
+    <row r="2">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Hello World</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Badland</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retrieve price on main and write on excel
Able to write on excel of the pricing of the products and check whether cell is occupied before writing it.
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -1,33 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvi\PycharmProjects\WebScrappingTool\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42FA3B6-71FB-42F7-AB05-06A2C914548D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5805" yWindow="1530" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="3720" yWindow="2970" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+  <si>
+    <t>This is Occupied</t>
+  </si>
+  <si>
+    <t>You have been juke</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +62,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -407,51 +364,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A12" sqref="A9:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello World</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Badland</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Hello World</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Badland</t>
-        </is>
-      </c>
-    </row>
-    <row r="4"/>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Test1</t>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write on the data on excel file by columns
Able to write to excel file by columns by the number of products in the list.

First row must have data in the excel sheet inside or else it would not be able to write in the excel file.
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvi\PycharmProjects\WebScrappingTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42FA3B6-71FB-42F7-AB05-06A2C914548D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D55AF1-67EC-4E51-8AB5-41BA5251A10E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2970" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
-  <si>
-    <t>This is Occupied</t>
-  </si>
-  <si>
-    <t>You have been juke</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="8">
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>$59.90</t>
+  </si>
+  <si>
+    <t>Hello there</t>
+  </si>
+  <si>
+    <t>Hello WhaaT?</t>
+  </si>
+  <si>
+    <t>$45.00</t>
+  </si>
+  <si>
+    <t>$219.0</t>
+  </si>
+  <si>
+    <t>$169.0</t>
+  </si>
+  <si>
+    <t>$39.90</t>
   </si>
 </sst>
 </file>
@@ -61,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,53 +384,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A9:A12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Merge if there is no big changes to the code
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2790" yWindow="825" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -416,60 +416,60 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="32.33203125" customWidth="1" min="2" max="2"/>
-    <col width="38.109375" customWidth="1" min="3" max="3"/>
+    <col width="32.28515625" customWidth="1" min="2" max="2"/>
+    <col width="38.140625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">Stanley 750ml Stainless Steel Classic Vacuum Flask Water Bottle 25oz Black For Road Trip Camping Fishing Outdoor </t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">Logitech MX Master 3 Advanced Wireless Mouse With Bluetooth, Ultra-Fast Magspeed Scroll, In App Customization and Pair up to 3 Devices (Work From Home, Home Based Learning) </t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">CETAPHIL GENTLE SKIN CLEANSER 1L </t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">SanDisk Ultra SD UHS-I U1 (Up to 80MB/s Read) Memory Card SDSDUNR (32GB / 64GB / 128GB / 256GB) </t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">STANLEY Cordless 18V Brushless Hammer Drill Driver SBH201D2K </t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">Xiaomi Mi Dual Mode Wireless Mouse Silent Edition </t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">Apple iPhone SE: Buy sell online Smartphones  with cheap price </t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">Apple iPhone SE: Buy sell online Smartphones  with cheap price </t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t xml:space="preserve">captcha </t>
+          <t xml:space="preserve">Apple iPhone SE: Buy sell online Smartphones  with cheap price </t>
         </is>
       </c>
     </row>
@@ -489,7 +489,36 @@
           <t>$39.90</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>$219.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>$29.90</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>$719.0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="n"/>

</xml_diff>

<commit_message>
Added Date of Extraction
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2790" yWindow="825" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -15,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -45,9 +48,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,112 +418,270 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="32.28515625" customWidth="1" min="2" max="2"/>
-    <col width="38.140625" customWidth="1" min="3" max="3"/>
+    <col width="104.85546875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="166" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="33.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="92.85546875" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="59.5703125" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="48.42578125" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="59.140625" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="59.140625" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="59.140625" bestFit="1" customWidth="1" min="19" max="19"/>
+    <col width="92.28515625" bestFit="1" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t xml:space="preserve">Stanley 750ml Stainless Steel Classic Vacuum Flask Water Bottle 25oz Black For Road Trip Camping Fishing Outdoor </t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t xml:space="preserve">Logitech MX Master 3 Advanced Wireless Mouse With Bluetooth, Ultra-Fast Magspeed Scroll, In App Customization and Pair up to 3 Devices (Work From Home, Home Based Learning) </t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t xml:space="preserve">CETAPHIL GENTLE SKIN CLEANSER 1L </t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t xml:space="preserve">SanDisk Ultra SD UHS-I U1 (Up to 80MB/s Read) Memory Card SDSDUNR (32GB / 64GB / 128GB / 256GB) </t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t xml:space="preserve">STANLEY Cordless 18V Brushless Hammer Drill Driver SBH201D2K </t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t xml:space="preserve">Xiaomi Mi Dual Mode Wireless Mouse Silent Edition </t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t xml:space="preserve">Apple iPhone SE: Buy sell online Smartphones  with cheap price </t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t xml:space="preserve">Apple iPhone SE: Buy sell online Smartphones  with cheap price </t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t xml:space="preserve">Apple iPhone SE: Buy sell online Smartphones  with cheap price </t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRISM+ X240 (1200R) 24 144Hz 1ms Curved FHD [1920 x 1080] FreeSync G-Sync Ready Gaming Monitor </t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>$59.90</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>$169.0</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>$39.90</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>$45.00</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>$219.0</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>$29.90</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>$889.0</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>$719.0</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>$889.0</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>$369.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$169.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>$219.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>$29.90</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>$719.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>$369.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$169.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>$219.0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>$29.90</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>$719.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>$369.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n"/>
     </row>
     <row r="19">
       <c r="B19" s="1" t="n"/>
@@ -526,4 +689,38 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16.140625" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>DATE EXTRACTED</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Mode of Extraction
Utilise Selenium as extraction mode.

Added debugging statement.
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,11 +49,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,25 +665,474 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n"/>
+      <c r="A5" s="3" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$169.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>$219.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>$29.90</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>$719.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>$369.0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n"/>
+      <c r="A6" s="3" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$169.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>$219.0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>$29.90</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>$719.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>$889.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>$369.0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n"/>
+      <c r="A7" s="3" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
+      <c r="A8" s="3" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>$709.00
+$719.00-1%</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n"/>
+      <c r="A9" s="3" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n"/>
+      <c r="A10" s="3" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>$709.00
+$719.00-1%</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n"/>
+      <c r="A11" s="3" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>$709.00
+$719.00-1%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>$709.00
+$719.00-1%</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="n"/>

</xml_diff>

<commit_message>
Added Selenium Searching into main
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -1134,6 +1134,121 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>44207</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>$24.90
+$29.90-17%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>$851.00
+$889.00-4%</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>$289.00
+$369.00-22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>44207</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>$59.90</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$169.00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$39.90</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>$219.00</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>$24.90</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>$851.00</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>$851.00</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>$851.00</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>$289.00</t>
+        </is>
+      </c>
+    </row>
     <row r="19">
       <c r="B19" s="1" t="n"/>
     </row>

</xml_diff>